<commit_message>
final submit & pdf generation
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -3,31 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -399,11 +393,11 @@
   </sheetPr>
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="12.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="51.21875" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -611,6 +605,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -633,6 +632,11 @@
           <t>8907097340.020X8</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>08907097173605</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>L091303</t>
@@ -701,6 +705,11 @@
       <c r="S3" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Success</t>
         </is>
       </c>
     </row>
@@ -725,6 +734,11 @@
           <t>8907097340.030XB</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>08907097173612</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>L091303</t>
@@ -793,6 +807,11 @@
       <c r="S4" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Success</t>
         </is>
       </c>
     </row>
@@ -817,6 +836,11 @@
           <t>8907097340.040XE</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>08907097173629</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>L091303</t>
@@ -885,6 +909,11 @@
       <c r="S5" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Success</t>
         </is>
       </c>
     </row>
@@ -909,6 +938,11 @@
           <t>8907097340.050XH</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>08907097173636</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>L091303</t>
@@ -977,6 +1011,11 @@
       <c r="S6" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Success</t>
         </is>
       </c>
     </row>

</xml_diff>